<commit_message>
maj excel apres ajout
</commit_message>
<xml_diff>
--- a/Projet.xlsx
+++ b/Projet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
   <si>
     <t>ControleurAdminListe</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Gestion BDD :</t>
   </si>
   <si>
-    <t>Recharge la page avec le message ajouté</t>
-  </si>
-  <si>
     <t>afficherLesListes()</t>
   </si>
   <si>
@@ -276,6 +273,15 @@
   </si>
   <si>
     <t>Affichage d'un item dans une liste</t>
+  </si>
+  <si>
+    <t>afficherListe($token, $no)</t>
+  </si>
+  <si>
+    <t>/afficherListePartage/:tokenPartage/:id</t>
+  </si>
+  <si>
+    <t>Partager une liste</t>
   </si>
 </sst>
 </file>
@@ -326,12 +332,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -615,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,11 +637,11 @@
     <col min="3" max="3" width="60.140625" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -658,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -666,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -678,13 +687,13 @@
         <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -692,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -704,13 +713,13 @@
         <v>24</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -718,25 +727,25 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -744,56 +753,53 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
@@ -811,15 +817,15 @@
         <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4">
         <v>6</v>
@@ -837,215 +843,215 @@
         <v>3</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="4">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" t="s">
+        <v>83</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G12" t="s">
-        <v>53</v>
+      <c r="G12" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
+        <v>75</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4">
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
+        <v>76</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4">
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
         <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>35</v>
@@ -1053,51 +1059,51 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4">
-        <v>21</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="4">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" t="s">
-        <v>61</v>
+        <v>20</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>18</v>
@@ -1107,23 +1113,23 @@
       <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="4">
-        <v>22</v>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>18</v>
@@ -1134,22 +1140,22 @@
         <v>5</v>
       </c>
       <c r="B20" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>18</v>
@@ -1157,25 +1163,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="B21" s="4">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>21</v>
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>62</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>18</v>
@@ -1183,51 +1189,51 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>28</v>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>14</v>
+        <v>77</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>35</v>
@@ -1235,53 +1241,79 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G26" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
         <v>36</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G27" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
         <v>37</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:I23">

</xml_diff>